<commit_message>
Static ploting, animation not functional
</commit_message>
<xml_diff>
--- a/targets/test1.xlsx
+++ b/targets/test1.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -386,7 +386,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>4.216448146018998</v>
+        <v>20.46315725008776</v>
       </c>
     </row>
     <row r="3">
@@ -397,7 +397,7 @@
         <v>1.1</v>
       </c>
       <c r="C3" t="n">
-        <v>-20.24374284913165</v>
+        <v>-8.871362001440087</v>
       </c>
     </row>
     <row r="4">
@@ -408,7 +408,7 @@
         <v>2.2</v>
       </c>
       <c r="C4" t="n">
-        <v>-3.813970353617749</v>
+        <v>6.803275573276045</v>
       </c>
     </row>
     <row r="5">
@@ -419,7 +419,7 @@
         <v>3.3</v>
       </c>
       <c r="C5" t="n">
-        <v>-2.194624978158555</v>
+        <v>-2.753470682257613</v>
       </c>
     </row>
     <row r="6">
@@ -430,7 +430,7 @@
         <v>4.4</v>
       </c>
       <c r="C6" t="n">
-        <v>-12.89604101366829</v>
+        <v>12.74719179615108</v>
       </c>
     </row>
     <row r="7">
@@ -441,7 +441,7 @@
         <v>5.5</v>
       </c>
       <c r="C7" t="n">
-        <v>11.50454270022955</v>
+        <v>-8.996605711510755</v>
       </c>
     </row>
     <row r="8">
@@ -452,7 +452,7 @@
         <v>6.6</v>
       </c>
       <c r="C8" t="n">
-        <v>-10.79111632704854</v>
+        <v>-4.853370001023103</v>
       </c>
     </row>
     <row r="9">
@@ -460,10 +460,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>7.7</v>
+        <v>7.699999999999999</v>
       </c>
       <c r="C9" t="n">
-        <v>7.349216666927934</v>
+        <v>-14.01748220980055</v>
       </c>
     </row>
     <row r="10">
@@ -471,10 +471,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>8.800000000000001</v>
+        <v>8.799999999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>-7.506494493506947</v>
+        <v>4.527168444763065</v>
       </c>
     </row>
     <row r="11">
@@ -482,10 +482,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>9.9</v>
+        <v>9.899999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.631409151974646</v>
+        <v>-5.391267436463464</v>
       </c>
     </row>
     <row r="12">
@@ -496,7 +496,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>19.02886110715081</v>
+        <v>9.690016386984103</v>
       </c>
     </row>
     <row r="13">
@@ -507,7 +507,7 @@
         <v>12.1</v>
       </c>
       <c r="C13" t="n">
-        <v>-26.61795915315089</v>
+        <v>5.939281940682445</v>
       </c>
     </row>
     <row r="14">
@@ -518,7 +518,7 @@
         <v>13.2</v>
       </c>
       <c r="C14" t="n">
-        <v>-8.184818533072239</v>
+        <v>-7.634711911220005</v>
       </c>
     </row>
     <row r="15">
@@ -529,7 +529,7 @@
         <v>14.3</v>
       </c>
       <c r="C15" t="n">
-        <v>5.627812674485989</v>
+        <v>-6.263356606729044</v>
       </c>
     </row>
     <row r="16">
@@ -540,7 +540,7 @@
         <v>15.4</v>
       </c>
       <c r="C16" t="n">
-        <v>9.18070164930376</v>
+        <v>0.932446025522675</v>
       </c>
     </row>
     <row r="17">
@@ -551,7 +551,7 @@
         <v>16.5</v>
       </c>
       <c r="C17" t="n">
-        <v>-17.06691563996162</v>
+        <v>0.7346028022933537</v>
       </c>
     </row>
     <row r="18">
@@ -562,7 +562,7 @@
         <v>17.6</v>
       </c>
       <c r="C18" t="n">
-        <v>-8.963673901882354</v>
+        <v>14.63082831826653</v>
       </c>
     </row>
     <row r="19">
@@ -573,7 +573,7 @@
         <v>18.7</v>
       </c>
       <c r="C19" t="n">
-        <v>13.88849456636381</v>
+        <v>6.912665085636519</v>
       </c>
     </row>
     <row r="20">
@@ -584,7 +584,7 @@
         <v>19.8</v>
       </c>
       <c r="C20" t="n">
-        <v>-8.670128235358828</v>
+        <v>-2.946189457186951</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>20.9</v>
       </c>
       <c r="C21" t="n">
-        <v>-6.705244815422457</v>
+        <v>-15.17831728192271</v>
       </c>
     </row>
     <row r="22">
@@ -606,7 +606,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="n">
-        <v>-10.09017910097756</v>
+        <v>9.34162203604075</v>
       </c>
     </row>
     <row r="23">
@@ -617,7 +617,7 @@
         <v>23.1</v>
       </c>
       <c r="C23" t="n">
-        <v>-11.93874269220428</v>
+        <v>1.74485536124526</v>
       </c>
     </row>
     <row r="24">
@@ -625,10 +625,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>24.2</v>
+        <v>24.20000000000001</v>
       </c>
       <c r="C24" t="n">
-        <v>-7.553636774778447</v>
+        <v>9.679005220521654</v>
       </c>
     </row>
     <row r="25">
@@ -636,10 +636,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>25.3</v>
+        <v>25.30000000000001</v>
       </c>
       <c r="C25" t="n">
-        <v>-7.000467474138925</v>
+        <v>-7.426001500536788</v>
       </c>
     </row>
     <row r="26">
@@ -647,10 +647,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>26.4</v>
+        <v>26.40000000000001</v>
       </c>
       <c r="C26" t="n">
-        <v>-15.76692938049085</v>
+        <v>10.98027960908465</v>
       </c>
     </row>
     <row r="27">
@@ -658,10 +658,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>27.5</v>
+        <v>27.50000000000001</v>
       </c>
       <c r="C27" t="n">
-        <v>-1.961058769513213</v>
+        <v>-12.64345235274561</v>
       </c>
     </row>
     <row r="28">
@@ -669,10 +669,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>28.6</v>
+        <v>28.60000000000001</v>
       </c>
       <c r="C28" t="n">
-        <v>8.371336461821706</v>
+        <v>-10.17970735623242</v>
       </c>
     </row>
     <row r="29">
@@ -680,10 +680,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>29.7</v>
+        <v>29.70000000000001</v>
       </c>
       <c r="C29" t="n">
-        <v>14.90725140729779</v>
+        <v>-1.787385927220983</v>
       </c>
     </row>
     <row r="30">
@@ -691,10 +691,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>30.8</v>
+        <v>30.80000000000001</v>
       </c>
       <c r="C30" t="n">
-        <v>-5.940782302735414</v>
+        <v>-14.82256042731548</v>
       </c>
     </row>
     <row r="31">
@@ -702,10 +702,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>31.9</v>
+        <v>31.90000000000002</v>
       </c>
       <c r="C31" t="n">
-        <v>-29.03879687722838</v>
+        <v>10.9447860140084</v>
       </c>
     </row>
     <row r="32">
@@ -713,10 +713,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>33</v>
+        <v>33.00000000000001</v>
       </c>
       <c r="C32" t="n">
-        <v>11.87138582423956</v>
+        <v>3.656340843174286</v>
       </c>
     </row>
     <row r="33">
@@ -724,10 +724,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>34.1</v>
+        <v>34.10000000000002</v>
       </c>
       <c r="C33" t="n">
-        <v>7.782110815393439</v>
+        <v>-0.2563721846741766</v>
       </c>
     </row>
     <row r="34">
@@ -735,10 +735,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>35.2</v>
+        <v>35.20000000000002</v>
       </c>
       <c r="C34" t="n">
-        <v>3.138469414659136</v>
+        <v>-7.661025087283079</v>
       </c>
     </row>
     <row r="35">
@@ -746,10 +746,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>36.3</v>
+        <v>36.30000000000002</v>
       </c>
       <c r="C35" t="n">
-        <v>13.59377966573341</v>
+        <v>-18.73522161967288</v>
       </c>
     </row>
     <row r="36">
@@ -757,10 +757,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>37.4</v>
+        <v>37.40000000000002</v>
       </c>
       <c r="C36" t="n">
-        <v>0.8675404694655777</v>
+        <v>-2.336404862798283</v>
       </c>
     </row>
     <row r="37">
@@ -768,10 +768,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>38.5</v>
+        <v>38.50000000000002</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.3334888891606677</v>
+        <v>-6.117131279581152</v>
       </c>
     </row>
     <row r="38">
@@ -779,10 +779,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>39.6</v>
+        <v>39.60000000000002</v>
       </c>
       <c r="C38" t="n">
-        <v>2.117323903385261</v>
+        <v>-10.57595917320752</v>
       </c>
     </row>
     <row r="39">
@@ -790,10 +790,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>40.7</v>
+        <v>40.70000000000002</v>
       </c>
       <c r="C39" t="n">
-        <v>-4.573376989926448</v>
+        <v>-5.504797896560647</v>
       </c>
     </row>
     <row r="40">
@@ -801,10 +801,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>41.8</v>
+        <v>41.80000000000003</v>
       </c>
       <c r="C40" t="n">
-        <v>13.87568485357357</v>
+        <v>-1.907095634737647</v>
       </c>
     </row>
     <row r="41">
@@ -812,10 +812,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>42.9</v>
+        <v>42.90000000000003</v>
       </c>
       <c r="C41" t="n">
-        <v>10.18946045047803</v>
+        <v>-4.054855616330562</v>
       </c>
     </row>
     <row r="42">
@@ -823,10 +823,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>44</v>
+        <v>44.00000000000003</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.1353314361135539</v>
+        <v>2.167677736431082</v>
       </c>
     </row>
     <row r="43">
@@ -834,10 +834,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>45.09999999999999</v>
+        <v>45.10000000000003</v>
       </c>
       <c r="C43" t="n">
-        <v>9.427792814786407</v>
+        <v>-14.61331937269333</v>
       </c>
     </row>
     <row r="44">
@@ -845,10 +845,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>46.2</v>
+        <v>46.20000000000003</v>
       </c>
       <c r="C44" t="n">
-        <v>-4.487550699294939</v>
+        <v>1.763213644053386</v>
       </c>
     </row>
     <row r="45">
@@ -856,10 +856,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>47.3</v>
+        <v>47.30000000000003</v>
       </c>
       <c r="C45" t="n">
-        <v>0.3524197770564022</v>
+        <v>-7.409518265668426</v>
       </c>
     </row>
     <row r="46">
@@ -867,10 +867,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>48.4</v>
+        <v>48.40000000000003</v>
       </c>
       <c r="C46" t="n">
-        <v>19.92033149065069</v>
+        <v>9.233460107240255</v>
       </c>
     </row>
     <row r="47">
@@ -878,10 +878,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>49.5</v>
+        <v>49.50000000000004</v>
       </c>
       <c r="C47" t="n">
-        <v>11.11606717753073</v>
+        <v>-3.10008851554772</v>
       </c>
     </row>
     <row r="48">
@@ -889,10 +889,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>50.6</v>
+        <v>50.60000000000004</v>
       </c>
       <c r="C48" t="n">
-        <v>-17.57536770551771</v>
+        <v>7.056147080660277</v>
       </c>
     </row>
     <row r="49">
@@ -900,10 +900,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>51.7</v>
+        <v>51.70000000000004</v>
       </c>
       <c r="C49" t="n">
-        <v>34.96899528829746</v>
+        <v>4.311363025421969</v>
       </c>
     </row>
     <row r="50">
@@ -911,10 +911,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>52.8</v>
+        <v>52.80000000000004</v>
       </c>
       <c r="C50" t="n">
-        <v>-9.086843695160898</v>
+        <v>-1.915697423997605</v>
       </c>
     </row>
     <row r="51">
@@ -922,10 +922,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>53.9</v>
+        <v>53.90000000000004</v>
       </c>
       <c r="C51" t="n">
-        <v>15.90663307960823</v>
+        <v>7.278561227610139</v>
       </c>
     </row>
     <row r="52">
@@ -933,10 +933,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>55</v>
+        <v>55.00000000000004</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.8424289409075965</v>
+        <v>2.319948216946591</v>
       </c>
     </row>
     <row r="53">
@@ -944,10 +944,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>56.1</v>
+        <v>56.10000000000004</v>
       </c>
       <c r="C53" t="n">
-        <v>7.230300156922337</v>
+        <v>-2.786791244652302</v>
       </c>
     </row>
     <row r="54">
@@ -955,10 +955,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>57.2</v>
+        <v>57.20000000000005</v>
       </c>
       <c r="C54" t="n">
-        <v>-4.171601808696285</v>
+        <v>-6.267557027072623</v>
       </c>
     </row>
     <row r="55">
@@ -966,10 +966,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>58.3</v>
+        <v>58.30000000000005</v>
       </c>
       <c r="C55" t="n">
-        <v>-2.03227688466585</v>
+        <v>-19.75759761966443</v>
       </c>
     </row>
     <row r="56">
@@ -977,10 +977,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>59.40000000000001</v>
+        <v>59.40000000000005</v>
       </c>
       <c r="C56" t="n">
-        <v>-6.086944932690724</v>
+        <v>13.41625513447663</v>
       </c>
     </row>
     <row r="57">
@@ -988,10 +988,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>60.50000000000001</v>
+        <v>60.50000000000005</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.3549283629160962</v>
+        <v>-7.91024938243501</v>
       </c>
     </row>
     <row r="58">
@@ -999,10 +999,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>61.6</v>
+        <v>61.60000000000005</v>
       </c>
       <c r="C58" t="n">
-        <v>2.22680921615165</v>
+        <v>-5.619680341410904</v>
       </c>
     </row>
     <row r="59">
@@ -1010,10 +1010,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>62.7</v>
+        <v>62.70000000000005</v>
       </c>
       <c r="C59" t="n">
-        <v>2.777214244854517</v>
+        <v>-5.631614546368065</v>
       </c>
     </row>
     <row r="60">
@@ -1021,10 +1021,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>63.8</v>
+        <v>63.80000000000005</v>
       </c>
       <c r="C60" t="n">
-        <v>15.03654602433498</v>
+        <v>-2.864770294520354</v>
       </c>
     </row>
     <row r="61">
@@ -1032,10 +1032,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>64.90000000000001</v>
+        <v>64.90000000000005</v>
       </c>
       <c r="C61" t="n">
-        <v>12.2092935620434</v>
+        <v>-2.165155831899343</v>
       </c>
     </row>
     <row r="62">
@@ -1043,10 +1043,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>66</v>
+        <v>66.00000000000004</v>
       </c>
       <c r="C62" t="n">
-        <v>-6.632892134303025</v>
+        <v>8.55312234478756</v>
       </c>
     </row>
     <row r="63">
@@ -1054,10 +1054,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>67.09999999999999</v>
+        <v>67.10000000000004</v>
       </c>
       <c r="C63" t="n">
-        <v>18.42705331469634</v>
+        <v>-10.50665060936482</v>
       </c>
     </row>
     <row r="64">
@@ -1065,10 +1065,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>68.19999999999999</v>
+        <v>68.20000000000003</v>
       </c>
       <c r="C64" t="n">
-        <v>-13.98500859919642</v>
+        <v>-6.559906776314818</v>
       </c>
     </row>
     <row r="65">
@@ -1076,10 +1076,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>69.3</v>
+        <v>69.30000000000003</v>
       </c>
       <c r="C65" t="n">
-        <v>13.33925609677995</v>
+        <v>-13.73044460349132</v>
       </c>
     </row>
     <row r="66">
@@ -1087,10 +1087,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>70.39999999999999</v>
+        <v>70.40000000000002</v>
       </c>
       <c r="C66" t="n">
-        <v>11.2764273376485</v>
+        <v>-7.113486767825908</v>
       </c>
     </row>
     <row r="67">
@@ -1098,10 +1098,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>71.5</v>
+        <v>71.50000000000001</v>
       </c>
       <c r="C67" t="n">
-        <v>-12.38623279422066</v>
+        <v>-0.6937881474173797</v>
       </c>
     </row>
     <row r="68">
@@ -1109,10 +1109,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>72.59999999999999</v>
+        <v>72.60000000000001</v>
       </c>
       <c r="C68" t="n">
-        <v>-3.160267396470995</v>
+        <v>-4.783216995699267</v>
       </c>
     </row>
     <row r="69">
@@ -1120,10 +1120,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>73.69999999999999</v>
+        <v>73.7</v>
       </c>
       <c r="C69" t="n">
-        <v>-8.588858503237546</v>
+        <v>1.018119696560815</v>
       </c>
     </row>
     <row r="70">
@@ -1134,7 +1134,7 @@
         <v>74.8</v>
       </c>
       <c r="C70" t="n">
-        <v>-0.9677766711297213</v>
+        <v>-5.532114454705477</v>
       </c>
     </row>
     <row r="71">
@@ -1145,7 +1145,7 @@
         <v>75.89999999999999</v>
       </c>
       <c r="C71" t="n">
-        <v>3.803198031546688</v>
+        <v>-6.881708503923551</v>
       </c>
     </row>
     <row r="72">
@@ -1153,10 +1153,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>77</v>
+        <v>76.99999999999999</v>
       </c>
       <c r="C72" t="n">
-        <v>-10.67452273451562</v>
+        <v>-10.06953039859076</v>
       </c>
     </row>
     <row r="73">
@@ -1164,10 +1164,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>78.09999999999999</v>
+        <v>78.09999999999998</v>
       </c>
       <c r="C73" t="n">
-        <v>-1.691485385737622</v>
+        <v>4.776997964709762</v>
       </c>
     </row>
     <row r="74">
@@ -1175,10 +1175,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>79.19999999999999</v>
+        <v>79.19999999999997</v>
       </c>
       <c r="C74" t="n">
-        <v>0.540763936079914</v>
+        <v>-10.317878486377</v>
       </c>
     </row>
     <row r="75">
@@ -1186,10 +1186,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>80.3</v>
+        <v>80.29999999999997</v>
       </c>
       <c r="C75" t="n">
-        <v>-14.25655851888139</v>
+        <v>-10.17673111843692</v>
       </c>
     </row>
     <row r="76">
@@ -1197,10 +1197,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>81.39999999999999</v>
+        <v>81.39999999999996</v>
       </c>
       <c r="C76" t="n">
-        <v>10.52756541662244</v>
+        <v>7.710533746143586</v>
       </c>
     </row>
     <row r="77">
@@ -1208,10 +1208,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>82.5</v>
+        <v>82.49999999999996</v>
       </c>
       <c r="C77" t="n">
-        <v>0.9554534893584525</v>
+        <v>-1.507901070348139</v>
       </c>
     </row>
     <row r="78">
@@ -1219,10 +1219,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>83.59999999999999</v>
+        <v>83.59999999999995</v>
       </c>
       <c r="C78" t="n">
-        <v>1.644576792132981</v>
+        <v>-1.113437540682142</v>
       </c>
     </row>
     <row r="79">
@@ -1230,10 +1230,10 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>84.7</v>
+        <v>84.69999999999995</v>
       </c>
       <c r="C79" t="n">
-        <v>13.24223056000071</v>
+        <v>-4.208875242643325</v>
       </c>
     </row>
     <row r="80">
@@ -1241,10 +1241,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>85.8</v>
+        <v>85.79999999999994</v>
       </c>
       <c r="C80" t="n">
-        <v>-15.68173667222121</v>
+        <v>-13.35408333101818</v>
       </c>
     </row>
     <row r="81">
@@ -1252,10 +1252,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>86.90000000000001</v>
+        <v>86.89999999999993</v>
       </c>
       <c r="C81" t="n">
-        <v>-2.739442739154244</v>
+        <v>2.438968470909062</v>
       </c>
     </row>
     <row r="82">
@@ -1263,10 +1263,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>88</v>
+        <v>87.99999999999993</v>
       </c>
       <c r="C82" t="n">
-        <v>14.81519149073537</v>
+        <v>-2.087409342912719</v>
       </c>
     </row>
     <row r="83">
@@ -1274,10 +1274,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>89.09999999999999</v>
+        <v>89.09999999999992</v>
       </c>
       <c r="C83" t="n">
-        <v>-6.560140171429541</v>
+        <v>6.747578769235247</v>
       </c>
     </row>
     <row r="84">
@@ -1285,10 +1285,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>90.2</v>
+        <v>90.19999999999992</v>
       </c>
       <c r="C84" t="n">
-        <v>-1.056420365386267</v>
+        <v>-8.558197192471734</v>
       </c>
     </row>
     <row r="85">
@@ -1296,10 +1296,318 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>91.3</v>
+        <v>91.29999999999991</v>
       </c>
       <c r="C85" t="n">
-        <v>-19.91999620104272</v>
+        <v>5.806552822150973</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>92.39999999999991</v>
+      </c>
+      <c r="C86" t="n">
+        <v>-7.048718900101809</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>93.4999999999999</v>
+      </c>
+      <c r="C87" t="n">
+        <v>-16.09709705985068</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="n">
+        <v>94.59999999999989</v>
+      </c>
+      <c r="C88" t="n">
+        <v>-16.14303247086716</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="n">
+        <v>95.69999999999989</v>
+      </c>
+      <c r="C89" t="n">
+        <v>1.449554180435693</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>96.79999999999988</v>
+      </c>
+      <c r="C90" t="n">
+        <v>8.330247609231924</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>97.89999999999988</v>
+      </c>
+      <c r="C91" t="n">
+        <v>8.58578527482352</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="n">
+        <v>98.99999999999987</v>
+      </c>
+      <c r="C92" t="n">
+        <v>4.435036605073154</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="n">
+        <v>100.0999999999999</v>
+      </c>
+      <c r="C93" t="n">
+        <v>-6.914884225776671</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="n">
+        <v>101.1999999999999</v>
+      </c>
+      <c r="C94" t="n">
+        <v>5.051340354079974</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="n">
+        <v>102.2999999999999</v>
+      </c>
+      <c r="C95" t="n">
+        <v>12.88220840161638</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="n">
+        <v>103.3999999999998</v>
+      </c>
+      <c r="C96" t="n">
+        <v>-2.553188231157454</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>104.4999999999998</v>
+      </c>
+      <c r="C97" t="n">
+        <v>11.89150616439616</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>105.5999999999998</v>
+      </c>
+      <c r="C98" t="n">
+        <v>9.587071702997644</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>106.6999999999998</v>
+      </c>
+      <c r="C99" t="n">
+        <v>-5.414525401398792</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>107.7999999999998</v>
+      </c>
+      <c r="C100" t="n">
+        <v>-13.11977186947088</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
+        <v>108.8999999999998</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0.7996134891376993</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="n">
+        <v>109.9999999999998</v>
+      </c>
+      <c r="C102" t="n">
+        <v>9.818744208345191</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="n">
+        <v>111.0999999999998</v>
+      </c>
+      <c r="C103" t="n">
+        <v>5.063682026918908</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="n">
+        <v>112.1999999999998</v>
+      </c>
+      <c r="C104" t="n">
+        <v>-11.75914295985498</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="n">
+        <v>113.2999999999998</v>
+      </c>
+      <c r="C105" t="n">
+        <v>-0.9397642029997761</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="n">
+        <v>114.3999999999998</v>
+      </c>
+      <c r="C106" t="n">
+        <v>-3.216744901127722</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="n">
+        <v>115.4999999999998</v>
+      </c>
+      <c r="C107" t="n">
+        <v>-11.20916337697438</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="n">
+        <v>116.5999999999998</v>
+      </c>
+      <c r="C108" t="n">
+        <v>6.617085102115009</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="n">
+        <v>117.6999999999998</v>
+      </c>
+      <c r="C109" t="n">
+        <v>-15.73650902978004</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="n">
+        <v>118.7999999999998</v>
+      </c>
+      <c r="C110" t="n">
+        <v>-4.224035879589111</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="n">
+        <v>119.8999999999998</v>
+      </c>
+      <c r="C111" t="n">
+        <v>-17.94925916833105</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="n">
+        <v>120.9999999999998</v>
+      </c>
+      <c r="C112" t="n">
+        <v>2.597982777644918</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="n">
+        <v>122.0999999999998</v>
+      </c>
+      <c r="C113" t="n">
+        <v>14.54918396463502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>